<commit_message>
sem casas decimais na percentagem
</commit_message>
<xml_diff>
--- a/Relatorio.xlsx
+++ b/Relatorio.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <workbookProtection workbookPassword="F7C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação" sheetId="1" r:id="rId1"/>
@@ -597,6 +597,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -623,27 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -993,7 +993,9 @@
       <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="22"/>
+      <c r="C2" s="22">
+        <v>59</v>
+      </c>
       <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1082,251 +1084,265 @@
       <c r="I8" s="21"/>
     </row>
     <row r="10" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="34"/>
+      <c r="I10" s="34"/>
     </row>
     <row r="11" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="35"/>
+      <c r="H11" s="35"/>
+      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="2:9" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="32"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
+      <c r="F12" s="37"/>
+      <c r="G12" s="37"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
     </row>
     <row r="13" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
     </row>
     <row r="14" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="34"/>
     </row>
     <row r="15" spans="2:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="34"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="36"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="36"/>
-      <c r="I16" s="35"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="27"/>
     </row>
     <row r="17" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
     </row>
     <row r="18" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="39"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
       <c r="I18" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="34" t="s">
+      <c r="B19" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="E19" s="34" t="s">
+      <c r="C19" s="27"/>
+      <c r="E19" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="35"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="27"/>
       <c r="H19" s="2"/>
       <c r="I19" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="E20" s="34" t="s">
+      <c r="C20" s="27"/>
+      <c r="E20" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="36"/>
-      <c r="G20" s="35"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="27"/>
       <c r="H20" s="2"/>
       <c r="I20" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="21" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="34" t="s">
+      <c r="B21" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="E21" s="34" t="s">
+      <c r="C21" s="27"/>
+      <c r="E21" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="36"/>
-      <c r="G21" s="35"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="2"/>
       <c r="I21" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="34" t="s">
+      <c r="B22" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="35"/>
-      <c r="E22" s="34" t="s">
+      <c r="C22" s="27"/>
+      <c r="E22" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="35"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="27"/>
       <c r="H22" s="2"/>
       <c r="I22" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="23" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="E23" s="34" t="s">
+      <c r="C23" s="27"/>
+      <c r="E23" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="36"/>
-      <c r="G23" s="35"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="27"/>
       <c r="H23" s="2"/>
       <c r="I23" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="24" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="35"/>
-      <c r="E24" s="34" t="s">
+      <c r="C24" s="27"/>
+      <c r="E24" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="35"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="27"/>
       <c r="H24" s="2"/>
       <c r="I24" s="23" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="E25" s="34" t="s">
+      <c r="C25" s="27"/>
+      <c r="E25" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="36"/>
-      <c r="G25" s="35"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="27"/>
       <c r="H25" s="2"/>
       <c r="I25" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="26" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="35"/>
-      <c r="E26" s="34" t="s">
+      <c r="C26" s="27"/>
+      <c r="E26" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="F26" s="36"/>
-      <c r="G26" s="35"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="27"/>
       <c r="H26" s="2"/>
       <c r="I26" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="34"/>
-      <c r="C27" s="35"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="35"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="2"/>
       <c r="I27" s="23"/>
     </row>
     <row r="28" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="34"/>
-      <c r="C28" s="35"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="35"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="27"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="27"/>
       <c r="H28" s="2"/>
       <c r="I28" s="23"/>
     </row>
   </sheetData>
   <sheetProtection password="F7C2" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="30">
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="E28:G28"/>
     <mergeCell ref="B18:C18"/>
@@ -1343,20 +1359,6 @@
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="E24:G24"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1367,7 +1369,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -1406,11 +1408,11 @@
       <c r="I3" s="41"/>
     </row>
     <row r="4" spans="2:9" s="11" customFormat="1" ht="195.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>

</xml_diff>

<commit_message>
descrição dos extras - relatorio
</commit_message>
<xml_diff>
--- a/Relatorio.xlsx
+++ b/Relatorio.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escola\Ainet\ainetproject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projetos\ainetproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookPassword="F7C2" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Identificação" sheetId="1" r:id="rId1"/>
@@ -374,7 +374,7 @@
     <t>Tem que se fazer composer install e php artisan passport: install.</t>
   </si>
   <si>
-    <t>Foi adicionado um sino de notificações para os administradores. (Mandar um mail para todos os administradores sempre que for criado um novo pedido.)</t>
+    <t>Foi incliudo suporte para "api calls" com o laravel passport o que possibilita apenas aos utilizadores autenticados aceder a determinada informação através de uma api. Para que os administradores terem noção do que se passa em tempo real foi adicionado um sistemas de notificações, (um sino na barra de menu com uma cor associado ao estado dos pedidos, azul - nenhum pedido, amarelo - pedidos em espera, vermelho pedidos expirados) que apresenta os ultimos pedidos adicionados que indicando se o pazo de entrega(due_date) foi ultrapassado ou não, também pode ser feita a filtragem por departamento. Sempre que um pedido for criado todos os adminitradores são notificados e poderam aceder ao pedido apenas à distância de um clique.</t>
   </si>
 </sst>
 </file>
@@ -597,6 +597,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -609,41 +636,14 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -973,23 +973,23 @@
       <selection activeCell="B12" sqref="B12:I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13" style="1" customWidth="1"/>
-    <col min="4" max="4" width="2.875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="2.8984375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.59765625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.59765625" style="1" customWidth="1"/>
     <col min="7" max="7" width="2.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="12.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="82.875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.875" style="1"/>
+    <col min="9" max="9" width="82.8984375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.8984375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
@@ -1000,16 +1000,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" ht="9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24"/>
       <c r="C4" s="24" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>1</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1049,7 +1049,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>1</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1083,268 +1083,254 @@
       </c>
       <c r="I8" s="21"/>
     </row>
-    <row r="10" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="34" t="s">
+    <row r="10" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-    </row>
-    <row r="11" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="35" t="s">
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+    </row>
+    <row r="11" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
-    </row>
-    <row r="12" spans="2:9" ht="138" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="36" t="s">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+    </row>
+    <row r="12" spans="2:9" ht="138" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="38"/>
-    </row>
-    <row r="13" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-    </row>
-    <row r="14" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="34" t="s">
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
+    </row>
+    <row r="13" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+    </row>
+    <row r="14" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-    </row>
-    <row r="15" spans="2:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="32" t="s">
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+    </row>
+    <row r="15" spans="2:9" ht="38.1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="33"/>
-      <c r="G15" s="33"/>
-      <c r="H15" s="33"/>
-      <c r="I15" s="33"/>
-    </row>
-    <row r="16" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
-      <c r="I16" s="27"/>
-    </row>
-    <row r="17" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+    </row>
+    <row r="16" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="34"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="35"/>
+    </row>
+    <row r="17" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-    </row>
-    <row r="18" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+    </row>
+    <row r="18" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="39"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="29" t="s">
+      <c r="E18" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
       <c r="I18" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+    <row r="19" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="E19" s="26" t="s">
+      <c r="C19" s="35"/>
+      <c r="E19" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="27"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="35"/>
       <c r="H19" s="2"/>
       <c r="I19" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
+    <row r="20" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="E20" s="26" t="s">
+      <c r="C20" s="35"/>
+      <c r="E20" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="27"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="35"/>
       <c r="H20" s="2"/>
       <c r="I20" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
+    <row r="21" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="E21" s="26" t="s">
+      <c r="C21" s="35"/>
+      <c r="E21" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="27"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="35"/>
       <c r="H21" s="2"/>
       <c r="I21" s="23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+    <row r="22" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="27"/>
-      <c r="E22" s="26" t="s">
+      <c r="C22" s="35"/>
+      <c r="E22" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="28"/>
-      <c r="G22" s="27"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="35"/>
       <c r="H22" s="2"/>
       <c r="I22" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="26" t="s">
+    <row r="23" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="E23" s="26" t="s">
+      <c r="C23" s="35"/>
+      <c r="E23" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="27"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="35"/>
       <c r="H23" s="2"/>
       <c r="I23" s="23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+    <row r="24" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="34" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="27"/>
-      <c r="E24" s="26" t="s">
+      <c r="C24" s="35"/>
+      <c r="E24" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="27"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="2"/>
       <c r="I24" s="23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="26" t="s">
+    <row r="25" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="E25" s="26" t="s">
+      <c r="C25" s="35"/>
+      <c r="E25" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F25" s="28"/>
-      <c r="G25" s="27"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="35"/>
       <c r="H25" s="2"/>
       <c r="I25" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="26" t="s">
+    <row r="26" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C26" s="27"/>
-      <c r="E26" s="26" t="s">
+      <c r="C26" s="35"/>
+      <c r="E26" s="34" t="s">
         <v>69</v>
       </c>
-      <c r="F26" s="28"/>
-      <c r="G26" s="27"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="35"/>
       <c r="H26" s="2"/>
       <c r="I26" s="23" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="26"/>
-      <c r="C27" s="27"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="27"/>
+    <row r="27" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="34"/>
+      <c r="C27" s="35"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="2"/>
       <c r="I27" s="23"/>
     </row>
-    <row r="28" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="26"/>
-      <c r="C28" s="27"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="27"/>
+    <row r="28" spans="2:9" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="34"/>
+      <c r="C28" s="35"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="35"/>
       <c r="H28" s="2"/>
       <c r="I28" s="23"/>
     </row>
   </sheetData>
   <sheetProtection password="F7C2" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="30">
-    <mergeCell ref="B15:I15"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="E20:G20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E21:G21"/>
-    <mergeCell ref="B16:I16"/>
-    <mergeCell ref="B17:I17"/>
-    <mergeCell ref="E19:G19"/>
-    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="E28:G28"/>
     <mergeCell ref="B18:C18"/>
@@ -1361,6 +1347,20 @@
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="E24:G24"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:G21"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="E19:G19"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -1371,21 +1371,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" style="12" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="12"/>
-    <col min="3" max="3" width="23.875" style="12" customWidth="1"/>
+    <col min="2" max="2" width="10.8984375" style="12"/>
+    <col min="3" max="3" width="23.8984375" style="12" customWidth="1"/>
     <col min="4" max="4" width="99.5" style="13" customWidth="1"/>
-    <col min="5" max="5" width="127.125" style="7" customWidth="1"/>
-    <col min="6" max="16384" width="10.875" style="12"/>
+    <col min="5" max="5" width="127.09765625" style="7" customWidth="1"/>
+    <col min="6" max="16384" width="10.8984375" style="12"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" s="11" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" s="11" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="40" t="s">
         <v>7</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="H2" s="40"/>
       <c r="I2" s="40"/>
     </row>
-    <row r="3" spans="2:9" s="11" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" s="11" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="41" t="s">
         <v>63</v>
       </c>
@@ -1409,19 +1409,19 @@
       <c r="H3" s="41"/>
       <c r="I3" s="41"/>
     </row>
-    <row r="4" spans="2:9" s="11" customFormat="1" ht="195.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+    <row r="4" spans="2:9" s="11" customFormat="1" ht="195.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="38"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="6" spans="2:9" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B6" s="42" t="s">
         <v>15</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
     </row>
-    <row r="8" spans="2:9" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" s="11" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="15" t="s">
         <v>1</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1459,7 +1459,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>17</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>18</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>19</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="5" t="s">
         <v>20</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="5" t="s">
         <v>21</v>
       </c>
@@ -1519,7 +1519,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1531,7 +1531,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="5" t="s">
         <v>23</v>
       </c>
@@ -1543,7 +1543,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="5" t="s">
         <v>24</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="5" t="s">
         <v>25</v>
       </c>
@@ -1567,7 +1567,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="5" t="s">
         <v>27</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="5" t="s">
         <v>28</v>
       </c>
@@ -1603,7 +1603,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="5" t="s">
         <v>29</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="5" t="s">
         <v>30</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="5" t="s">
         <v>31</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="5" t="s">
         <v>32</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="5" t="s">
         <v>33</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="5" t="s">
         <v>34</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5" t="s">
         <v>35</v>
       </c>
@@ -1687,7 +1687,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B29" s="5" t="s">
         <v>36</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" s="10" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
         <v>37</v>
       </c>
@@ -1711,183 +1711,183 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D31" s="13"/>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D32" s="13"/>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D33" s="13"/>
       <c r="E33" s="8"/>
     </row>
-    <row r="34" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D34" s="13"/>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D35" s="13"/>
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D36" s="13"/>
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D37" s="13"/>
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D38" s="13"/>
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D39" s="13"/>
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D40" s="13"/>
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:5" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D41" s="13"/>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E46" s="9"/>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E47" s="9"/>
     </row>
-    <row r="48" spans="4:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:5" x14ac:dyDescent="0.3">
       <c r="E48" s="9"/>
     </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" s="9"/>
     </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E50" s="9"/>
     </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E51" s="9"/>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" s="9"/>
     </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" s="9"/>
     </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" s="9"/>
     </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E55" s="9"/>
     </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E56" s="9"/>
     </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E57" s="9"/>
     </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E58" s="9"/>
     </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E59" s="9"/>
     </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E60" s="9"/>
     </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E61" s="9"/>
     </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E62" s="9"/>
     </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E63" s="9"/>
     </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E64" s="9"/>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E65" s="9"/>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E66" s="9"/>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E67" s="9"/>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E68" s="9"/>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E69" s="9"/>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E70" s="9"/>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E71" s="9"/>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E72" s="9"/>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E73" s="9"/>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E74" s="9"/>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E75" s="9"/>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E76" s="9"/>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E77" s="9"/>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E78" s="9"/>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E79" s="9"/>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E80" s="9"/>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E81" s="9"/>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E82" s="9"/>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E83" s="9"/>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E84" s="9"/>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E85" s="9"/>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E86" s="9"/>
     </row>
   </sheetData>

</xml_diff>